<commit_message>
se arreglan diferencias sutiles con silber 93-04
</commit_message>
<xml_diff>
--- a/results/enge_results.xlsx
+++ b/results/enge_results.xlsx
@@ -4281,7 +4281,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>44826.4</v>
+        <v>29991</v>
       </c>
       <c r="E53" t="n">
         <v>568814</v>
@@ -4308,37 +4308,37 @@
         <v>0.5068669474</v>
       </c>
       <c r="M53" t="n">
-        <v>64736.57328133199</v>
+        <v>43311.85572074554</v>
       </c>
       <c r="N53" t="n">
-        <v>88438.19907756723</v>
+        <v>59169.37404153174</v>
       </c>
       <c r="O53" t="n">
-        <v>24517.92972981664</v>
+        <v>16403.66459334077</v>
       </c>
       <c r="P53" t="n">
-        <v>44826.4</v>
+        <v>29991</v>
       </c>
       <c r="Q53" t="n">
-        <v>1.693308407079984</v>
+        <v>1.132904101974189</v>
       </c>
       <c r="R53" t="n">
         <v>1.098111364439288</v>
       </c>
       <c r="S53" t="n">
-        <v>0.1138097397063574</v>
+        <v>0.07614414504696709</v>
       </c>
       <c r="T53" t="n">
-        <v>0.155478239068601</v>
+        <v>0.1040223588757164</v>
       </c>
       <c r="U53" t="n">
-        <v>0.04310359753771292</v>
+        <v>0.02883836296810693</v>
       </c>
       <c r="V53" t="n">
-        <v>0.07880678042382923</v>
+        <v>0.05272549550468167</v>
       </c>
       <c r="W53" t="n">
-        <v>1.542018835170341</v>
+        <v>1.031684161244126</v>
       </c>
     </row>
     <row r="54">
@@ -7785,10 +7785,10 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>17872</v>
+        <v>17963.8</v>
       </c>
       <c r="E101" t="n">
-        <v>107690</v>
+        <v>107749</v>
       </c>
       <c r="F101" t="n">
         <v>1</v>
@@ -7812,37 +7812,37 @@
         <v>1</v>
       </c>
       <c r="M101" t="n">
-        <v>17872</v>
+        <v>17963.8</v>
       </c>
       <c r="N101" t="n">
-        <v>17872</v>
+        <v>17963.8</v>
       </c>
       <c r="O101" t="n">
-        <v>5068.171950656996</v>
+        <v>5094.204749732103</v>
       </c>
       <c r="P101" t="n">
-        <v>6099.658703071672</v>
+        <v>6130.98976109215</v>
       </c>
       <c r="Q101" t="n">
-        <v>1.516709961357638</v>
+        <v>1.524500582130502</v>
       </c>
       <c r="R101" t="n">
-        <v>1.021668595715614</v>
+        <v>1.022228336147847</v>
       </c>
       <c r="S101" t="n">
-        <v>0.1659578419537562</v>
+        <v>0.166718948667737</v>
       </c>
       <c r="T101" t="n">
-        <v>0.1659578419537562</v>
+        <v>0.166718948667737</v>
       </c>
       <c r="U101" t="n">
-        <v>0.04706260516906859</v>
+        <v>0.04727844109673503</v>
       </c>
       <c r="V101" t="n">
-        <v>0.05664090169070175</v>
+        <v>0.05690066507431298</v>
       </c>
       <c r="W101" t="n">
-        <v>1.48454202049274</v>
+        <v>1.491350345340075</v>
       </c>
     </row>
     <row r="102">
@@ -7858,10 +7858,10 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>20475</v>
+        <v>20152.1</v>
       </c>
       <c r="E102" t="n">
-        <v>41394</v>
+        <v>41785</v>
       </c>
       <c r="F102" t="n">
         <v>1</v>
@@ -7885,37 +7885,37 @@
         <v>1</v>
       </c>
       <c r="M102" t="n">
-        <v>20475</v>
+        <v>20152.1</v>
       </c>
       <c r="N102" t="n">
-        <v>20475</v>
+        <v>20152.1</v>
       </c>
       <c r="O102" t="n">
-        <v>5806.335087830237</v>
+        <v>5714.766560364528</v>
       </c>
       <c r="P102" t="n">
-        <v>6988.054607508532</v>
+        <v>6877.849829351535</v>
       </c>
       <c r="Q102" t="n">
-        <v>1.310262691868615</v>
+        <v>1.289599257279878</v>
       </c>
       <c r="R102" t="n">
-        <v>0.8601708122934979</v>
+        <v>0.8682958252810506</v>
       </c>
       <c r="S102" t="n">
-        <v>0.4946369038991158</v>
+        <v>0.4822807227473974</v>
       </c>
       <c r="T102" t="n">
-        <v>0.4946369038991158</v>
+        <v>0.4822807227473974</v>
       </c>
       <c r="U102" t="n">
-        <v>0.1402699687836459</v>
+        <v>0.1367659820596991</v>
       </c>
       <c r="V102" t="n">
-        <v>0.1688180559382648</v>
+        <v>0.1646009292653233</v>
       </c>
       <c r="W102" t="n">
-        <v>1.523258721573014</v>
+        <v>1.48520725279597</v>
       </c>
     </row>
     <row r="103">
@@ -7931,10 +7931,10 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>8254</v>
+        <v>8250</v>
       </c>
       <c r="E103" t="n">
-        <v>56356</v>
+        <v>56424</v>
       </c>
       <c r="F103" t="n">
         <v>1</v>
@@ -7958,37 +7958,37 @@
         <v>1</v>
       </c>
       <c r="M103" t="n">
-        <v>8254</v>
+        <v>8250</v>
       </c>
       <c r="N103" t="n">
-        <v>8254</v>
+        <v>8250</v>
       </c>
       <c r="O103" t="n">
-        <v>2340.683263245459</v>
+        <v>2339.548936488374</v>
       </c>
       <c r="P103" t="n">
-        <v>2817.064846416382</v>
+        <v>2815.699658703072</v>
       </c>
       <c r="Q103" t="n">
-        <v>0.7567611690461101</v>
+        <v>0.7563944323516366</v>
       </c>
       <c r="R103" t="n">
-        <v>0.9492336196732356</v>
+        <v>0.9503789792824658</v>
       </c>
       <c r="S103" t="n">
-        <v>0.146461778692597</v>
+        <v>0.1462143768609102</v>
       </c>
       <c r="T103" t="n">
-        <v>0.146461778692597</v>
+        <v>0.1462143768609102</v>
       </c>
       <c r="U103" t="n">
-        <v>0.04153387861532861</v>
+        <v>0.04146371998597004</v>
       </c>
       <c r="V103" t="n">
-        <v>0.04998695518518671</v>
+        <v>0.04990251769996937</v>
       </c>
       <c r="W103" t="n">
-        <v>0.7972338456644822</v>
+        <v>0.7958871658995581</v>
       </c>
     </row>
     <row r="104">
@@ -8004,10 +8004,10 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>5609</v>
+        <v>5608.1</v>
       </c>
       <c r="E104" t="n">
-        <v>30300</v>
+        <v>30290</v>
       </c>
       <c r="F104" t="n">
         <v>1</v>
@@ -8031,37 +8031,37 @@
         <v>1</v>
       </c>
       <c r="M104" t="n">
-        <v>5609</v>
+        <v>5608.1</v>
       </c>
       <c r="N104" t="n">
-        <v>5609</v>
+        <v>5608.1</v>
       </c>
       <c r="O104" t="n">
-        <v>1590.609695122823</v>
+        <v>1590.354471602479</v>
       </c>
       <c r="P104" t="n">
-        <v>1914.334470989761</v>
+        <v>1914.027303754266</v>
       </c>
       <c r="Q104" t="n">
-        <v>0.7809588668933612</v>
+        <v>0.7808335570377357</v>
       </c>
       <c r="R104" t="n">
-        <v>0.9384872700241591</v>
+        <v>0.9381775382518739</v>
       </c>
       <c r="S104" t="n">
-        <v>0.1851155115511551</v>
+        <v>0.1851469131726643</v>
       </c>
       <c r="T104" t="n">
-        <v>0.1851155115511551</v>
+        <v>0.1851469131726643</v>
       </c>
       <c r="U104" t="n">
-        <v>0.05249536947600076</v>
+        <v>0.05250427440087418</v>
       </c>
       <c r="V104" t="n">
-        <v>0.06317935547820994</v>
+        <v>0.06319007275517552</v>
       </c>
       <c r="W104" t="n">
-        <v>0.8321464678719162</v>
+        <v>0.8322876270227909</v>
       </c>
     </row>
     <row r="105">
@@ -8077,10 +8077,10 @@
         </is>
       </c>
       <c r="D105" t="n">
-        <v>3071</v>
+        <v>3155.9</v>
       </c>
       <c r="E105" t="n">
-        <v>23441</v>
+        <v>23412</v>
       </c>
       <c r="F105" t="n">
         <v>1</v>
@@ -8104,37 +8104,37 @@
         <v>1</v>
       </c>
       <c r="M105" t="n">
-        <v>3071</v>
+        <v>3155.9</v>
       </c>
       <c r="N105" t="n">
-        <v>3071</v>
+        <v>3155.9</v>
       </c>
       <c r="O105" t="n">
-        <v>870.8793677522177</v>
+        <v>894.9554531713527</v>
       </c>
       <c r="P105" t="n">
-        <v>1048.122866894198</v>
+        <v>1077.098976109215</v>
       </c>
       <c r="Q105" t="n">
-        <v>0.6665090759592626</v>
+        <v>0.6849351979224476</v>
       </c>
       <c r="R105" t="n">
-        <v>0.5624715056988602</v>
+        <v>0.5617756448710258</v>
       </c>
       <c r="S105" t="n">
-        <v>0.1310097692077983</v>
+        <v>0.1347983939859901</v>
       </c>
       <c r="T105" t="n">
-        <v>0.1310097692077983</v>
+        <v>0.1347983939859901</v>
       </c>
       <c r="U105" t="n">
-        <v>0.03715197166299295</v>
+        <v>0.03822635627760775</v>
       </c>
       <c r="V105" t="n">
-        <v>0.04471323181153525</v>
+        <v>0.04600627781091812</v>
       </c>
       <c r="W105" t="n">
-        <v>1.184965050151541</v>
+        <v>1.21923263170246</v>
       </c>
     </row>
     <row r="106">
@@ -8150,7 +8150,7 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>24500</v>
+        <v>24455.2</v>
       </c>
       <c r="E106" t="n">
         <v>18315</v>
@@ -8177,37 +8177,37 @@
         <v>1</v>
       </c>
       <c r="M106" t="n">
-        <v>24500</v>
+        <v>24455.2</v>
       </c>
       <c r="N106" t="n">
-        <v>24500</v>
+        <v>24455.2</v>
       </c>
       <c r="O106" t="n">
-        <v>6947.751387147292</v>
+        <v>6935.046927467937</v>
       </c>
       <c r="P106" t="n">
-        <v>8361.774744027303</v>
+        <v>8346.484641638224</v>
       </c>
       <c r="Q106" t="n">
-        <v>2.591876434051874</v>
+        <v>2.587137002858179</v>
       </c>
       <c r="R106" t="n">
         <v>1.536751132740393</v>
       </c>
       <c r="S106" t="n">
-        <v>1.337701337701338</v>
+        <v>1.335255255255255</v>
       </c>
       <c r="T106" t="n">
-        <v>1.337701337701338</v>
+        <v>1.335255255255255</v>
       </c>
       <c r="U106" t="n">
-        <v>0.3793476050858473</v>
+        <v>0.3786539408936903</v>
       </c>
       <c r="V106" t="n">
-        <v>0.4565533575772484</v>
+        <v>0.4557185171519642</v>
       </c>
       <c r="W106" t="n">
-        <v>1.686594777015028</v>
+        <v>1.6835107179942</v>
       </c>
     </row>
     <row r="107">
@@ -8223,10 +8223,10 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>48871</v>
+        <v>48973.5</v>
       </c>
       <c r="E107" t="n">
-        <v>546659</v>
+        <v>546163</v>
       </c>
       <c r="F107" t="n">
         <v>1</v>
@@ -8250,37 +8250,37 @@
         <v>1</v>
       </c>
       <c r="M107" t="n">
-        <v>48871</v>
+        <v>48973.5</v>
       </c>
       <c r="N107" t="n">
-        <v>48871</v>
+        <v>48973.5</v>
       </c>
       <c r="O107" t="n">
-        <v>13858.92073637858</v>
+        <v>13887.9878595289</v>
       </c>
       <c r="P107" t="n">
-        <v>16679.52218430034</v>
+        <v>16714.50511945392</v>
       </c>
       <c r="Q107" t="n">
-        <v>0.9357232058719835</v>
+        <v>0.9376857527525851</v>
       </c>
       <c r="R107" t="n">
-        <v>1.055340516184582</v>
+        <v>1.054382974287297</v>
       </c>
       <c r="S107" t="n">
-        <v>0.08939942450412414</v>
+        <v>0.08966828584140632</v>
       </c>
       <c r="T107" t="n">
-        <v>0.08939942450412414</v>
+        <v>0.08966828584140632</v>
       </c>
       <c r="U107" t="n">
-        <v>0.02535203982076319</v>
+        <v>0.02542828397296942</v>
       </c>
       <c r="V107" t="n">
-        <v>0.03051174897751677</v>
+        <v>0.03060351052607724</v>
       </c>
       <c r="W107" t="n">
-        <v>0.8866552468344001</v>
+        <v>0.8893217887802174</v>
       </c>
     </row>
     <row r="108">
@@ -8296,10 +8296,10 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>102857</v>
+        <v>102721.4</v>
       </c>
       <c r="E108" t="n">
-        <v>536217</v>
+        <v>536407</v>
       </c>
       <c r="F108" t="n">
         <v>1</v>
@@ -8323,37 +8323,37 @@
         <v>1</v>
       </c>
       <c r="M108" t="n">
-        <v>102857</v>
+        <v>102721.4</v>
       </c>
       <c r="N108" t="n">
-        <v>102857</v>
+        <v>102721.4</v>
       </c>
       <c r="O108" t="n">
-        <v>29168.36181337996</v>
+        <v>29129.90813631477</v>
       </c>
       <c r="P108" t="n">
-        <v>35104.77815699659</v>
+        <v>35058.49829351535</v>
       </c>
       <c r="Q108" t="n">
-        <v>1.280725793722465</v>
+        <v>1.279037367872705</v>
       </c>
       <c r="R108" t="n">
-        <v>0.9792469059372038</v>
+        <v>0.9795938865665537</v>
       </c>
       <c r="S108" t="n">
-        <v>0.1918197296989838</v>
+        <v>0.1914989923695999</v>
       </c>
       <c r="T108" t="n">
-        <v>0.1918197296989838</v>
+        <v>0.1914989923695999</v>
       </c>
       <c r="U108" t="n">
-        <v>0.05439656298360544</v>
+        <v>0.0543056077499264</v>
       </c>
       <c r="V108" t="n">
-        <v>0.06546748453890233</v>
+        <v>0.06535801787358358</v>
       </c>
       <c r="W108" t="n">
-        <v>1.307868103496049</v>
+        <v>1.30568124751747</v>
       </c>
     </row>
     <row r="109">
@@ -8369,10 +8369,10 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>52562</v>
+        <v>52429.3</v>
       </c>
       <c r="E109" t="n">
-        <v>229966</v>
+        <v>230361</v>
       </c>
       <c r="F109" t="n">
         <v>1</v>
@@ -8396,37 +8396,37 @@
         <v>1</v>
       </c>
       <c r="M109" t="n">
-        <v>52562</v>
+        <v>52429.3</v>
       </c>
       <c r="N109" t="n">
-        <v>52562</v>
+        <v>52429.3</v>
       </c>
       <c r="O109" t="n">
-        <v>14905.62075147902</v>
+        <v>14867.98946131272</v>
       </c>
       <c r="P109" t="n">
-        <v>17939.24914675768</v>
+        <v>17893.9590443686</v>
       </c>
       <c r="Q109" t="n">
-        <v>1.334627713088638</v>
+        <v>1.331258261821052</v>
       </c>
       <c r="R109" t="n">
-        <v>0.862999253207642</v>
+        <v>0.8644815797472915</v>
       </c>
       <c r="S109" t="n">
-        <v>0.2285642225372446</v>
+        <v>0.2275962511015319</v>
       </c>
       <c r="T109" t="n">
-        <v>0.2285642225372446</v>
+        <v>0.2275962511015319</v>
       </c>
       <c r="U109" t="n">
-        <v>0.06481662833409731</v>
+        <v>0.06454212935919151</v>
       </c>
       <c r="V109" t="n">
-        <v>0.07800826707755788</v>
+        <v>0.07767790139984025</v>
       </c>
       <c r="W109" t="n">
-        <v>1.546499267673781</v>
+        <v>1.539949830059086</v>
       </c>
     </row>
     <row r="110">
@@ -10851,7 +10851,7 @@
         </is>
       </c>
       <c r="D143" t="n">
-        <v>112451</v>
+        <v>112450</v>
       </c>
       <c r="E143" t="n">
         <v>709084</v>
@@ -10878,37 +10878,37 @@
         <v>1.584837389</v>
       </c>
       <c r="M143" t="n">
-        <v>61881.47188786977</v>
+        <v>61880.92159065686</v>
       </c>
       <c r="N143" t="n">
-        <v>70954.28261630949</v>
+        <v>70953.65163674846</v>
       </c>
       <c r="O143" t="n">
-        <v>20195.87399469035</v>
+        <v>20195.69439758588</v>
       </c>
       <c r="P143" t="n">
-        <v>35326.77103513273</v>
+        <v>35326.45688255929</v>
       </c>
       <c r="Q143" t="n">
-        <v>1.358547375745941</v>
+        <v>1.358535294507217</v>
       </c>
       <c r="R143" t="n">
         <v>1.368906529624918</v>
       </c>
       <c r="S143" t="n">
-        <v>0.08726959272507878</v>
+        <v>0.08726881665734507</v>
       </c>
       <c r="T143" t="n">
-        <v>0.1000647068842471</v>
+        <v>0.1000638170326061</v>
       </c>
       <c r="U143" t="n">
-        <v>0.02848163827514138</v>
+        <v>0.02848138499470568</v>
       </c>
       <c r="V143" t="n">
-        <v>0.04982029073443023</v>
+        <v>0.04981984769443295</v>
       </c>
       <c r="W143" t="n">
-        <v>0.9924325338108985</v>
+        <v>0.9924237083443946</v>
       </c>
     </row>
     <row r="144">
@@ -12165,7 +12165,7 @@
         </is>
       </c>
       <c r="D161" t="n">
-        <v>174377</v>
+        <v>174376</v>
       </c>
       <c r="E161" t="n">
         <v>784440</v>
@@ -12192,37 +12192,37 @@
         <v>2.133751782</v>
       </c>
       <c r="M161" t="n">
-        <v>68035.17209161911</v>
+        <v>68034.78193023261</v>
       </c>
       <c r="N161" t="n">
-        <v>81723.18892526178</v>
+        <v>81722.72026718804</v>
       </c>
       <c r="O161" t="n">
-        <v>22463.7743125369</v>
+        <v>22463.64548950225</v>
       </c>
       <c r="P161" t="n">
-        <v>44826.99228791774</v>
+        <v>44826.735218509</v>
       </c>
       <c r="Q161" t="n">
-        <v>1.564737458517889</v>
+        <v>1.564728485216028</v>
       </c>
       <c r="R161" t="n">
         <v>1.514383399003461</v>
       </c>
       <c r="S161" t="n">
-        <v>0.08673088074501442</v>
+        <v>0.08673038336932412</v>
       </c>
       <c r="T161" t="n">
-        <v>0.1041802928525595</v>
+        <v>0.1041796954097038</v>
       </c>
       <c r="U161" t="n">
-        <v>0.02863670173950449</v>
+        <v>0.0286365375165752</v>
       </c>
       <c r="V161" t="n">
-        <v>0.05714521478751433</v>
+        <v>0.05714488707677961</v>
       </c>
       <c r="W161" t="n">
-        <v>1.033250535860049</v>
+        <v>1.033244610476908</v>
       </c>
     </row>
     <row r="162">

</xml_diff>